<commit_message>
changes done on pom.xml
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/TestData.xlsx
+++ b/target/test-classes/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\DCPLProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE7FCB3-070D-4276-87B3-C4EB2198A9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9D56A8-928C-4BE2-BF41-A5574B770672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="177">
   <si>
     <t>hrms_id</t>
   </si>
@@ -560,7 +560,10 @@
     <t>cashierpassword</t>
   </si>
   <si>
-    <t>31</t>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1370,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D04161-DFF8-4095-A5EB-FA021B973EF1}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection sqref="A1:BP2"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1967,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,22 +2012,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2128,22 +2131,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -2402,13 +2405,13 @@
         <v>62</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -2447,13 +2450,13 @@
         <v>76</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Z2" s="13" t="s">
         <v>87</v>
@@ -2519,13 +2522,13 @@
         <v>119</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="AV2" s="2" t="s">
         <v>129</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>127</v>

</xml_diff>